<commit_message>
upgrade mac version to 1.6.0.0
</commit_message>
<xml_diff>
--- a/data/xlsx/access.xlsx
+++ b/data/xlsx/access.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jww/Developer/python/terraformer/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C56A46-99F0-2048-A5C5-5630E2C11F22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37D6930-F17F-D74F-B81E-72A7D0822584}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="520" windowWidth="25600" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="25600" windowHeight="14760" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="aclheaders" sheetId="62" r:id="rId1"/>
@@ -207,9 +207,6 @@
     <t>md5</t>
   </si>
   <si>
-    <t>3des</t>
-  </si>
-  <si>
     <t>disabled</t>
   </si>
   <si>
@@ -244,6 +241,9 @@
   </si>
   <si>
     <t>udp</t>
+  </si>
+  <si>
+    <t>aes256</t>
   </si>
 </sst>
 </file>
@@ -343,9 +343,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -696,6 +693,9 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -738,149 +738,149 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{039F5A72-2E04-E045-9C9A-D435D378174B}" name="*name" dataDxfId="81"/>
     <tableColumn id="2" xr3:uid="{7818DB98-2599-904B-BA0F-0790B6E1B3E4}" name="*vpc" dataDxfId="80"/>
-    <tableColumn id="3" xr3:uid="{885D5470-5652-6B41-BA7D-CFCDAB5E5093}" name="resource_group" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{885D5470-5652-6B41-BA7D-CFCDAB5E5093}" name="resource_group" dataDxfId="79"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0501486B-99D9-D847-9265-3A1B8C4F9CB7}" name="Table32" displayName="Table32" ref="A1:B3" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0501486B-99D9-D847-9265-3A1B8C4F9CB7}" name="Table32" displayName="Table32" ref="A1:B3" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="A1:B3" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{2B5EBF30-5208-5D4D-BE48-42C200D7DA49}" name="*name" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{593C94B9-EB1B-0945-A6EA-29933D3679F2}" name="tags" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{2B5EBF30-5208-5D4D-BE48-42C200D7DA49}" name="*name" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{593C94B9-EB1B-0945-A6EA-29933D3679F2}" name="tags" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8524F582-25D9-D64B-A9C7-4FF4A27248B3}" name="Table1" displayName="Table1" ref="A1:M4" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8524F582-25D9-D64B-A9C7-4FF4A27248B3}" name="Table1" displayName="Table1" ref="A1:M4" totalsRowShown="0" headerRowDxfId="78" dataDxfId="77">
   <autoFilter ref="A1:M4" xr:uid="{00881A37-2AAB-7345-9099-83242FC8EDEA}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{36FEA897-58B8-8244-BBD2-F934FDEC8E9A}" name="*name" dataDxfId="77"/>
-    <tableColumn id="6" xr3:uid="{C499C2EF-3238-4B4A-8017-492B9A1A77FF}" name="*acl" dataDxfId="76"/>
-    <tableColumn id="2" xr3:uid="{F12A4B82-233E-A440-B918-86C5E4C82FD9}" name="*action" dataDxfId="75"/>
-    <tableColumn id="3" xr3:uid="{568185F1-B557-2C49-B724-A15618F6D5DE}" name="*source" dataDxfId="74"/>
-    <tableColumn id="4" xr3:uid="{F5A78E34-0750-6E4E-BE76-F9B327F65E12}" name="*destination" dataDxfId="73"/>
-    <tableColumn id="5" xr3:uid="{83261B25-C691-8D45-8989-863A46F2510F}" name="*direction" dataDxfId="72"/>
-    <tableColumn id="14" xr3:uid="{BF39CD2E-14E9-4A43-A8D3-BBB3BB29D4E4}" name="protocol" dataDxfId="71"/>
-    <tableColumn id="8" xr3:uid="{45AA1E0E-A6AB-7A46-B4AF-E99B2D4AD91B}" name="icmp_code" dataDxfId="70"/>
-    <tableColumn id="7" xr3:uid="{8C6CB998-6DD3-6047-8D31-AF31736ECC78}" name="icmp_type" dataDxfId="69"/>
-    <tableColumn id="10" xr3:uid="{5AAB00B2-E1E7-9E40-98F1-D7B64B119564}" name="port_min" dataDxfId="68"/>
-    <tableColumn id="9" xr3:uid="{61B251A9-3DF1-3543-868E-D48BC0D2FBE8}" name="port_max" dataDxfId="67"/>
-    <tableColumn id="12" xr3:uid="{DA76B0C3-0D2A-2C42-A980-F1A40B9E72F2}" name="source_port_min" dataDxfId="66"/>
-    <tableColumn id="11" xr3:uid="{DA919A14-BC6E-5547-A993-1B7855521094}" name="source_port_max" dataDxfId="65"/>
+    <tableColumn id="1" xr3:uid="{36FEA897-58B8-8244-BBD2-F934FDEC8E9A}" name="*name" dataDxfId="76"/>
+    <tableColumn id="6" xr3:uid="{C499C2EF-3238-4B4A-8017-492B9A1A77FF}" name="*acl" dataDxfId="75"/>
+    <tableColumn id="2" xr3:uid="{F12A4B82-233E-A440-B918-86C5E4C82FD9}" name="*action" dataDxfId="74"/>
+    <tableColumn id="3" xr3:uid="{568185F1-B557-2C49-B724-A15618F6D5DE}" name="*source" dataDxfId="73"/>
+    <tableColumn id="4" xr3:uid="{F5A78E34-0750-6E4E-BE76-F9B327F65E12}" name="*destination" dataDxfId="72"/>
+    <tableColumn id="5" xr3:uid="{83261B25-C691-8D45-8989-863A46F2510F}" name="*direction" dataDxfId="71"/>
+    <tableColumn id="14" xr3:uid="{BF39CD2E-14E9-4A43-A8D3-BBB3BB29D4E4}" name="protocol" dataDxfId="70"/>
+    <tableColumn id="8" xr3:uid="{45AA1E0E-A6AB-7A46-B4AF-E99B2D4AD91B}" name="icmp_code" dataDxfId="69"/>
+    <tableColumn id="7" xr3:uid="{8C6CB998-6DD3-6047-8D31-AF31736ECC78}" name="icmp_type" dataDxfId="68"/>
+    <tableColumn id="10" xr3:uid="{5AAB00B2-E1E7-9E40-98F1-D7B64B119564}" name="port_min" dataDxfId="67"/>
+    <tableColumn id="9" xr3:uid="{61B251A9-3DF1-3543-868E-D48BC0D2FBE8}" name="port_max" dataDxfId="66"/>
+    <tableColumn id="12" xr3:uid="{DA76B0C3-0D2A-2C42-A980-F1A40B9E72F2}" name="source_port_min" dataDxfId="65"/>
+    <tableColumn id="11" xr3:uid="{DA919A14-BC6E-5547-A993-1B7855521094}" name="source_port_max" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{83144CBC-65AD-804B-B36C-148A65E84D16}" name="Table184" displayName="Table184" ref="A1:C3" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{83144CBC-65AD-804B-B36C-148A65E84D16}" name="Table184" displayName="Table184" ref="A1:C3" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
   <autoFilter ref="A1:C3" xr:uid="{EF08DB4E-0002-F047-8599-404D4BBF8940}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{A724ADCC-F039-0D45-9937-58B50BC5715E}" name="*name" dataDxfId="62"/>
-    <tableColumn id="2" xr3:uid="{B9D7A6DC-911D-B749-AE7A-2DC2D907D356}" name="*vpc" dataDxfId="61"/>
-    <tableColumn id="3" xr3:uid="{CE9B4557-50B5-2A4A-AA03-F9F781F4F349}" name="resource_group" dataDxfId="60"/>
+    <tableColumn id="1" xr3:uid="{A724ADCC-F039-0D45-9937-58B50BC5715E}" name="*name" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{B9D7A6DC-911D-B749-AE7A-2DC2D907D356}" name="*vpc" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{CE9B4557-50B5-2A4A-AA03-F9F781F4F349}" name="resource_group" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{11008CC8-5C85-3B48-82BD-CD830AD3D6DF}" name="Table18" displayName="Table18" ref="A1:J6" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{11008CC8-5C85-3B48-82BD-CD830AD3D6DF}" name="Table18" displayName="Table18" ref="A1:J6" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
   <autoFilter ref="A1:J6" xr:uid="{EF08DB4E-0002-F047-8599-404D4BBF8940}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{203C77A6-285B-124C-AF24-A3511F6244F7}" name="*name" dataDxfId="57"/>
-    <tableColumn id="5" xr3:uid="{2F8C3C4B-0E49-4A4D-AC20-F814AA26DD74}" name="*group" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{42DAC7A2-384A-144A-9BDC-F241D22F7F74}" name="*direction" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{41DCA0FA-BF94-6343-BF46-01D165299C09}" name="*remote" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{15B7721A-4EE3-9847-9C27-38416048A9AE}" name="ip_version" dataDxfId="53"/>
-    <tableColumn id="11" xr3:uid="{FE5D1059-98EB-6246-BC1E-22FD29D3D313}" name="protocol" dataDxfId="52"/>
-    <tableColumn id="9" xr3:uid="{0C37575C-3952-904A-B11D-84DC7EE12B0F}" name="icmp_code" dataDxfId="51"/>
-    <tableColumn id="8" xr3:uid="{1CDA1E92-4A45-E742-B2ED-4B8D9670CA18}" name="icmp_type" dataDxfId="50"/>
-    <tableColumn id="7" xr3:uid="{DEE8533C-7DBB-6B4E-95DA-ADF92BBA34C8}" name="port_min" dataDxfId="49"/>
-    <tableColumn id="6" xr3:uid="{9B67B5CE-A552-3B4B-A870-AA27F074FBE8}" name="port_max" dataDxfId="48"/>
+    <tableColumn id="1" xr3:uid="{203C77A6-285B-124C-AF24-A3511F6244F7}" name="*name" dataDxfId="56"/>
+    <tableColumn id="5" xr3:uid="{2F8C3C4B-0E49-4A4D-AC20-F814AA26DD74}" name="*group" dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{42DAC7A2-384A-144A-9BDC-F241D22F7F74}" name="*direction" dataDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{41DCA0FA-BF94-6343-BF46-01D165299C09}" name="*remote" dataDxfId="53"/>
+    <tableColumn id="4" xr3:uid="{15B7721A-4EE3-9847-9C27-38416048A9AE}" name="ip_version" dataDxfId="52"/>
+    <tableColumn id="11" xr3:uid="{FE5D1059-98EB-6246-BC1E-22FD29D3D313}" name="protocol" dataDxfId="51"/>
+    <tableColumn id="9" xr3:uid="{0C37575C-3952-904A-B11D-84DC7EE12B0F}" name="icmp_code" dataDxfId="50"/>
+    <tableColumn id="8" xr3:uid="{1CDA1E92-4A45-E742-B2ED-4B8D9670CA18}" name="icmp_type" dataDxfId="49"/>
+    <tableColumn id="7" xr3:uid="{DEE8533C-7DBB-6B4E-95DA-ADF92BBA34C8}" name="port_min" dataDxfId="48"/>
+    <tableColumn id="6" xr3:uid="{9B67B5CE-A552-3B4B-A870-AA27F074FBE8}" name="port_max" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D0CA34BD-A489-B54D-8D4B-B907D54F9FC9}" name="Table3" displayName="Table3" ref="A1:D3" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D0CA34BD-A489-B54D-8D4B-B907D54F9FC9}" name="Table3" displayName="Table3" ref="A1:D3" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
   <autoFilter ref="A1:D3" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{FC67A5D3-A34E-3D4E-9E86-D02090ED17CB}" name="*name" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{F56C754B-0F5D-694F-BD5D-7925CDFC5F97}" name="*public_key" dataDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{FDE02962-4673-2D4C-AFB9-1D7FCFCC6AA0}" name="resource_group" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{79F1DE46-3AC5-284E-8E48-AA0D55380DFD}" name="tags" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{FC67A5D3-A34E-3D4E-9E86-D02090ED17CB}" name="*name" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{F56C754B-0F5D-694F-BD5D-7925CDFC5F97}" name="*public_key" dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{FDE02962-4673-2D4C-AFB9-1D7FCFCC6AA0}" name="resource_group" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{79F1DE46-3AC5-284E-8E48-AA0D55380DFD}" name="tags" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{74F9BE67-E011-B34A-A492-0717499F0410}" name="Table16" displayName="Table16" ref="A1:C3" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{74F9BE67-E011-B34A-A492-0717499F0410}" name="Table16" displayName="Table16" ref="A1:C3" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
   <autoFilter ref="A1:C3" xr:uid="{6D379596-E186-C240-BBB4-B8E74F1D3D56}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{5FD29999-A9F5-C549-98A3-DFD2B1437449}" name="*name" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{35CF1270-9B78-4243-98F7-E702702F38FF}" name="*subnet" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{B806F889-718F-584A-ADDF-8A3AD802CDFB}" name="resource_group" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{5FD29999-A9F5-C549-98A3-DFD2B1437449}" name="*name" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{35CF1270-9B78-4243-98F7-E702702F38FF}" name="*subnet" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{B806F889-718F-584A-ADDF-8A3AD802CDFB}" name="resource_group" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B4318CDD-C98E-1341-88CD-5334A857D418}" name="Table15" displayName="Table15" ref="A1:M3" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B4318CDD-C98E-1341-88CD-5334A857D418}" name="Table15" displayName="Table15" ref="A1:M3" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="A1:M3" xr:uid="{27D8B65D-C3AF-BD4B-8BB7-5754C974B57F}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{C4B8842B-2BB7-EB49-B6D2-B6721C54DC5F}" name="*name" dataDxfId="34"/>
-    <tableColumn id="13" xr3:uid="{78EC6C87-C780-E34D-BBD5-54ED244AB6D6}" name="*vpn_gateway" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{DBBB9AC2-20E7-974C-935D-20C40D819A02}" name="*peer_address" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{5CDA888D-9763-CE46-98E3-D4B85974B5A5}" name="*preshared_key" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{D1C2C80B-E944-E049-AD39-98867623465E}" name="local_cidrs" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{B6F5AA94-6774-DA4F-8D22-7820C9CFB052}" name="peer_cidrs" dataDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{A49490F8-FF19-4247-A9DC-3E9A8C9508D2}" name="admin_state_up" dataDxfId="28"/>
-    <tableColumn id="7" xr3:uid="{D393C6C1-4F72-964B-9D76-BE2A1539821D}" name="dead_peer_action" dataDxfId="27"/>
-    <tableColumn id="8" xr3:uid="{D523FCFB-A055-084E-B6ED-C788AB1D158E}" name="dead_peer_interval" dataDxfId="26"/>
-    <tableColumn id="9" xr3:uid="{9A0739C3-7687-E94A-984F-5C145DFE3E89}" name="dead_peer_timeout" dataDxfId="25"/>
-    <tableColumn id="10" xr3:uid="{ACD56801-B98E-7847-85C3-F2FFBA76F061}" name="ike_policy" dataDxfId="24"/>
-    <tableColumn id="11" xr3:uid="{1BD10945-B68C-DF4E-AA5E-ACEC66F06E3C}" name="ipsec_policy" dataDxfId="23"/>
-    <tableColumn id="12" xr3:uid="{4B0694AF-1BD1-694F-90B1-B1A9567550B0}" name="delete_timeout" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{C4B8842B-2BB7-EB49-B6D2-B6721C54DC5F}" name="*name" dataDxfId="33"/>
+    <tableColumn id="13" xr3:uid="{78EC6C87-C780-E34D-BBD5-54ED244AB6D6}" name="*vpn_gateway" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{DBBB9AC2-20E7-974C-935D-20C40D819A02}" name="*peer_address" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{5CDA888D-9763-CE46-98E3-D4B85974B5A5}" name="*preshared_key" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{D1C2C80B-E944-E049-AD39-98867623465E}" name="local_cidrs" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{B6F5AA94-6774-DA4F-8D22-7820C9CFB052}" name="peer_cidrs" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{A49490F8-FF19-4247-A9DC-3E9A8C9508D2}" name="admin_state_up" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{D393C6C1-4F72-964B-9D76-BE2A1539821D}" name="dead_peer_action" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{D523FCFB-A055-084E-B6ED-C788AB1D158E}" name="dead_peer_interval" dataDxfId="25"/>
+    <tableColumn id="9" xr3:uid="{9A0739C3-7687-E94A-984F-5C145DFE3E89}" name="dead_peer_timeout" dataDxfId="24"/>
+    <tableColumn id="10" xr3:uid="{ACD56801-B98E-7847-85C3-F2FFBA76F061}" name="ike_policy" dataDxfId="23"/>
+    <tableColumn id="11" xr3:uid="{1BD10945-B68C-DF4E-AA5E-ACEC66F06E3C}" name="ipsec_policy" dataDxfId="22"/>
+    <tableColumn id="12" xr3:uid="{4B0694AF-1BD1-694F-90B1-B1A9567550B0}" name="delete_timeout" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{48612795-253E-2045-9A1C-B75C9BF5816E}" name="Table111" displayName="Table111" ref="A1:F3" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{48612795-253E-2045-9A1C-B75C9BF5816E}" name="Table111" displayName="Table111" ref="A1:F3" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A1:F3" xr:uid="{00881A37-2AAB-7345-9099-83242FC8EDEA}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{73198180-EC4B-3448-8FD7-AD7FE682C21E}" name="*name" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{A3F85132-9C0A-074A-AD1C-FC8C58C48C9A}" name="*authentication_algorithm" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{E34718FD-92F0-1A43-80D5-70140F486148}" name="*encryption_algorithm" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{42FD0836-3534-9647-8D8D-7A54E0E1C7AA}" name="*pfs" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{59778D38-F5AC-AC4E-845F-BC7470387817}" name="key_lifetime" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{BABC3429-E57A-4F47-92E7-58CB470AF7F9}" name="resource_group" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{73198180-EC4B-3448-8FD7-AD7FE682C21E}" name="*name" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{A3F85132-9C0A-074A-AD1C-FC8C58C48C9A}" name="*authentication_algorithm" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{E34718FD-92F0-1A43-80D5-70140F486148}" name="*encryption_algorithm" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{42FD0836-3534-9647-8D8D-7A54E0E1C7AA}" name="*pfs" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{59778D38-F5AC-AC4E-845F-BC7470387817}" name="key_lifetime" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{BABC3429-E57A-4F47-92E7-58CB470AF7F9}" name="resource_group" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{EE4FC002-D07C-9447-9703-8452CE1C018E}" name="Table11112" displayName="Table11112" ref="A1:G3" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{EE4FC002-D07C-9447-9703-8452CE1C018E}" name="Table11112" displayName="Table11112" ref="A1:G3" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A1:G3" xr:uid="{00881A37-2AAB-7345-9099-83242FC8EDEA}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{06812B35-A623-5241-A8DF-8EEB6166846D}" name="*name" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{9551CB52-166F-6E47-9A17-EC3E828FEB2C}" name="*authentication_algorithm" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{246BA229-88CD-0A4B-AD52-5F86AA06873E}" name="*encryption_algorithm" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{2E993777-DA48-4C4D-B929-49BFFB90F9D0}" name="*dh_group" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{A6127979-DB02-954A-BE3A-277928AF4686}" name="ike_version" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{1E691E85-EB8B-A64D-B4A6-22E7A68094F6}" name="key_lifetime" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{9B4820A8-622D-1540-A53E-6FCBAB87C546}" name="resource_group" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{06812B35-A623-5241-A8DF-8EEB6166846D}" name="*name" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{9551CB52-166F-6E47-9A17-EC3E828FEB2C}" name="*authentication_algorithm" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{246BA229-88CD-0A4B-AD52-5F86AA06873E}" name="*encryption_algorithm" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{2E993777-DA48-4C4D-B929-49BFFB90F9D0}" name="*dh_group" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{A6127979-DB02-954A-BE3A-277928AF4686}" name="ike_version" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{1E691E85-EB8B-A64D-B4A6-22E7A68094F6}" name="key_lifetime" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{9B4820A8-622D-1540-A53E-6FCBAB87C546}" name="resource_group" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1151,7 +1151,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{515B7804-FA89-F84C-8321-3F26CCBED84F}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1270,22 +1270,22 @@
         <v>5</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -1308,7 +1308,7 @@
         <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -1341,7 +1341,7 @@
         <v>8</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -1475,16 +1475,16 @@
         <v>5</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -1502,7 +1502,7 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -1528,7 +1528,7 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1908,10 +1908,10 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="E2" s="1">
         <v>3600</v>
@@ -1938,7 +1938,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74C836A2-0C93-8B42-8C00-3FFAF090CB9E}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1957,10 +1959,10 @@
         <v>53</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>55</v>
@@ -1971,13 +1973,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="D2" s="1">
         <v>2</v>

</xml_diff>

<commit_message>
upgraded to version 1.11.0.1
</commit_message>
<xml_diff>
--- a/data/xlsx/access.xlsx
+++ b/data/xlsx/access.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jww/Developer/python/terraformer/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA273476-6301-EF46-AD8A-5DB3BDD9C0D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E1D638-5B78-0941-8165-5560A49F37FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5700" yWindow="1320" windowWidth="30440" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2620" yWindow="1820" windowWidth="30440" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="aclrules" sheetId="51" r:id="rId1"/>
@@ -20,8 +20,10 @@
     <sheet name="ikepolicies" sheetId="61" r:id="rId5"/>
     <sheet name="vpngateways" sheetId="63" r:id="rId6"/>
     <sheet name="vpnconnections" sheetId="64" r:id="rId7"/>
-    <sheet name="sshkeys" sheetId="65" r:id="rId8"/>
-    <sheet name="resourcegroups" sheetId="62" r:id="rId9"/>
+    <sheet name="transitgateways" sheetId="66" r:id="rId8"/>
+    <sheet name="transitconnections" sheetId="67" r:id="rId9"/>
+    <sheet name="sshkeys" sheetId="65" r:id="rId10"/>
+    <sheet name="resourcegroups" sheetId="62" r:id="rId11"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="189">
   <si>
     <t>*name</t>
   </si>
@@ -582,6 +584,24 @@
   </si>
   <si>
     <t>"${var.vpc-name}-dbtier-ssh-traffic"</t>
+  </si>
+  <si>
+    <t>*global</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>*gateway</t>
+  </si>
+  <si>
+    <t>*network_type</t>
+  </si>
+  <si>
+    <t>network_id</t>
   </si>
 </sst>
 </file>
@@ -670,94 +690,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="110">
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="128">
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -829,6 +762,9 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -872,32 +808,12 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="4"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -931,6 +847,16 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -997,6 +923,7 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1042,6 +969,197 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1128,173 +1246,205 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8524F582-25D9-D64B-A9C7-4FF4A27248B3}" name="Table1" displayName="Table1" ref="A1:T29" totalsRowShown="0" headerRowDxfId="109" dataDxfId="108">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8524F582-25D9-D64B-A9C7-4FF4A27248B3}" name="Table1" displayName="Table1" ref="A1:T29" totalsRowShown="0" headerRowDxfId="127" dataDxfId="126">
   <autoFilter ref="A1:T29" xr:uid="{00881A37-2AAB-7345-9099-83242FC8EDEA}"/>
   <tableColumns count="20">
-    <tableColumn id="6" xr3:uid="{5F01EE41-D9A5-0C49-B223-FECA253E39FA}" name="*file" dataDxfId="107"/>
-    <tableColumn id="13" xr3:uid="{6512E223-BE63-604E-9E99-E8695934A4DF}" name="*resource" dataDxfId="106"/>
-    <tableColumn id="1" xr3:uid="{36FEA897-58B8-8244-BBD2-F934FDEC8E9A}" name="*name" dataDxfId="105"/>
-    <tableColumn id="11" xr3:uid="{33249652-A343-474E-88A1-EE232BCB846D}" name="*vpc" dataDxfId="104"/>
-    <tableColumn id="14" xr3:uid="{79D5F4EF-1FF5-F543-9806-4A2F23C7321E}" name="resource_group" dataDxfId="103"/>
-    <tableColumn id="2" xr3:uid="{F12A4B82-233E-A440-B918-86C5E4C82FD9}" name="*action" dataDxfId="102"/>
-    <tableColumn id="3" xr3:uid="{568185F1-B557-2C49-B724-A15618F6D5DE}" name="*source" dataDxfId="101"/>
-    <tableColumn id="4" xr3:uid="{F5A78E34-0750-6E4E-BE76-F9B327F65E12}" name="*destination" dataDxfId="100"/>
-    <tableColumn id="5" xr3:uid="{83261B25-C691-8D45-8989-863A46F2510F}" name="*direction" dataDxfId="99"/>
-    <tableColumn id="8" xr3:uid="{45AA1E0E-A6AB-7A46-B4AF-E99B2D4AD91B}" name="icmp.code" dataDxfId="98"/>
-    <tableColumn id="7" xr3:uid="{8C6CB998-6DD3-6047-8D31-AF31736ECC78}" name="icmp.type" dataDxfId="97"/>
-    <tableColumn id="10" xr3:uid="{5AAB00B2-E1E7-9E40-98F1-D7B64B119564}" name="tcp.port_min" dataDxfId="96"/>
-    <tableColumn id="9" xr3:uid="{61B251A9-3DF1-3543-868E-D48BC0D2FBE8}" name="tcp.port_max" dataDxfId="95"/>
-    <tableColumn id="12" xr3:uid="{DA76B0C3-0D2A-2C42-A980-F1A40B9E72F2}" name="tcp.source_port_min" dataDxfId="94"/>
-    <tableColumn id="15" xr3:uid="{0EDE2D95-BAB9-7945-9134-960231125C9B}" name="tcp.source_port_max" dataDxfId="93"/>
-    <tableColumn id="16" xr3:uid="{6DFF4708-A270-C642-8599-823B3429D646}" name="udp.port_min" dataDxfId="92"/>
-    <tableColumn id="17" xr3:uid="{F9BF1CC2-8F1D-F545-94C9-6F62C4CCAB5B}" name="udp.port_max" dataDxfId="91"/>
-    <tableColumn id="18" xr3:uid="{58858423-AE14-EC4F-A48F-CB7D921E919A}" name="udp.source_port_min" dataDxfId="90"/>
-    <tableColumn id="19" xr3:uid="{96522931-CF7D-3244-886B-2845B7421637}" name="udp.source_port_max" dataDxfId="89"/>
-    <tableColumn id="20" xr3:uid="{8FBB7238-9ED7-EC40-A097-D6453EE8C74B}" name="comments" dataDxfId="88"/>
+    <tableColumn id="6" xr3:uid="{5F01EE41-D9A5-0C49-B223-FECA253E39FA}" name="*file" dataDxfId="125"/>
+    <tableColumn id="13" xr3:uid="{6512E223-BE63-604E-9E99-E8695934A4DF}" name="*resource" dataDxfId="124"/>
+    <tableColumn id="1" xr3:uid="{36FEA897-58B8-8244-BBD2-F934FDEC8E9A}" name="*name" dataDxfId="123"/>
+    <tableColumn id="11" xr3:uid="{33249652-A343-474E-88A1-EE232BCB846D}" name="*vpc" dataDxfId="122"/>
+    <tableColumn id="14" xr3:uid="{79D5F4EF-1FF5-F543-9806-4A2F23C7321E}" name="resource_group" dataDxfId="121"/>
+    <tableColumn id="2" xr3:uid="{F12A4B82-233E-A440-B918-86C5E4C82FD9}" name="*action" dataDxfId="120"/>
+    <tableColumn id="3" xr3:uid="{568185F1-B557-2C49-B724-A15618F6D5DE}" name="*source" dataDxfId="119"/>
+    <tableColumn id="4" xr3:uid="{F5A78E34-0750-6E4E-BE76-F9B327F65E12}" name="*destination" dataDxfId="118"/>
+    <tableColumn id="5" xr3:uid="{83261B25-C691-8D45-8989-863A46F2510F}" name="*direction" dataDxfId="117"/>
+    <tableColumn id="8" xr3:uid="{45AA1E0E-A6AB-7A46-B4AF-E99B2D4AD91B}" name="icmp.code" dataDxfId="116"/>
+    <tableColumn id="7" xr3:uid="{8C6CB998-6DD3-6047-8D31-AF31736ECC78}" name="icmp.type" dataDxfId="115"/>
+    <tableColumn id="10" xr3:uid="{5AAB00B2-E1E7-9E40-98F1-D7B64B119564}" name="tcp.port_min" dataDxfId="114"/>
+    <tableColumn id="9" xr3:uid="{61B251A9-3DF1-3543-868E-D48BC0D2FBE8}" name="tcp.port_max" dataDxfId="113"/>
+    <tableColumn id="12" xr3:uid="{DA76B0C3-0D2A-2C42-A980-F1A40B9E72F2}" name="tcp.source_port_min" dataDxfId="112"/>
+    <tableColumn id="15" xr3:uid="{0EDE2D95-BAB9-7945-9134-960231125C9B}" name="tcp.source_port_max" dataDxfId="111"/>
+    <tableColumn id="16" xr3:uid="{6DFF4708-A270-C642-8599-823B3429D646}" name="udp.port_min" dataDxfId="110"/>
+    <tableColumn id="17" xr3:uid="{F9BF1CC2-8F1D-F545-94C9-6F62C4CCAB5B}" name="udp.port_max" dataDxfId="109"/>
+    <tableColumn id="18" xr3:uid="{58858423-AE14-EC4F-A48F-CB7D921E919A}" name="udp.source_port_min" dataDxfId="108"/>
+    <tableColumn id="19" xr3:uid="{96522931-CF7D-3244-886B-2845B7421637}" name="udp.source_port_max" dataDxfId="107"/>
+    <tableColumn id="20" xr3:uid="{8FBB7238-9ED7-EC40-A097-D6453EE8C74B}" name="comments" dataDxfId="106"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{66B01468-17B1-DF49-BD45-B84826DE910D}" name="Table32" displayName="Table32" ref="A1:G4" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+  <autoFilter ref="A1:G4" xr:uid="{E53C9C86-FACA-2C40-85AF-B9BA3559B380}"/>
+  <tableColumns count="7">
+    <tableColumn id="6" xr3:uid="{8F21586E-BECB-3F45-BEAA-A449A14BE047}" name="*file" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{4EF03EBF-5996-424F-93A5-4447C7F1B426}" name="*resource" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{C065294C-9139-324E-B19B-962D20BC4BE9}" name="*name" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{592C42FA-35FC-334C-9912-6BAE32344BD6}" name="*public_key" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{A36A827B-73DB-0749-B08B-5E9FBF4CF71C}" name="resource_group" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{F6CE2A63-DCA4-AB46-AD6C-B729704A5EAC}" name="tags" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{461DC722-A60D-2D4E-8D06-0C3D76DA4F10}" name="comments" dataDxfId="25"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E8C732A8-0017-264D-8362-11409D4ADB8A}" name="Table329" displayName="Table329" ref="A1:E5" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+  <autoFilter ref="A1:E5" xr:uid="{853761A8-3C8D-D146-AF16-A9CD69B737CB}"/>
+  <tableColumns count="5">
+    <tableColumn id="6" xr3:uid="{C7B59D49-52B4-E74B-980A-CBAA1960F9B9}" name="*file" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{0F8D8265-8F60-6746-958A-BB70EE098749}" name="*resource" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{20125E38-3425-9540-8E50-F8247EA67681}" name="*name" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{50B39641-31D5-1A42-A833-F3F591AE4879}" name="tags" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{E9307884-D588-8840-BA44-7ABC5CDEF259}" name="comments" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{83144CBC-65AD-804B-B36C-148A65E84D16}" name="Table184" displayName="Table184" ref="A1:F7" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{83144CBC-65AD-804B-B36C-148A65E84D16}" name="Table184" displayName="Table184" ref="A1:F7" totalsRowShown="0" headerRowDxfId="105" dataDxfId="104">
   <autoFilter ref="A1:F7" xr:uid="{EF08DB4E-0002-F047-8599-404D4BBF8940}"/>
   <tableColumns count="6">
-    <tableColumn id="5" xr3:uid="{5D3AB5BE-1930-A549-B919-A59B94A9C99A}" name="*file" dataDxfId="85"/>
-    <tableColumn id="4" xr3:uid="{FEA1D7FA-4673-B347-ABB1-AB4F2DC35543}" name="*resource" dataDxfId="84"/>
-    <tableColumn id="1" xr3:uid="{A724ADCC-F039-0D45-9937-58B50BC5715E}" name="*name" dataDxfId="83"/>
-    <tableColumn id="2" xr3:uid="{B9D7A6DC-911D-B749-AE7A-2DC2D907D356}" name="*vpc" dataDxfId="82"/>
-    <tableColumn id="3" xr3:uid="{CE9B4557-50B5-2A4A-AA03-F9F781F4F349}" name="resource_group" dataDxfId="81"/>
-    <tableColumn id="6" xr3:uid="{88C1D531-D327-1544-A671-C5F07A82F946}" name="comments" dataDxfId="80"/>
+    <tableColumn id="5" xr3:uid="{5D3AB5BE-1930-A549-B919-A59B94A9C99A}" name="*file" dataDxfId="103"/>
+    <tableColumn id="4" xr3:uid="{FEA1D7FA-4673-B347-ABB1-AB4F2DC35543}" name="*resource" dataDxfId="102"/>
+    <tableColumn id="1" xr3:uid="{A724ADCC-F039-0D45-9937-58B50BC5715E}" name="*name" dataDxfId="101"/>
+    <tableColumn id="2" xr3:uid="{B9D7A6DC-911D-B749-AE7A-2DC2D907D356}" name="*vpc" dataDxfId="100"/>
+    <tableColumn id="3" xr3:uid="{CE9B4557-50B5-2A4A-AA03-F9F781F4F349}" name="resource_group" dataDxfId="99"/>
+    <tableColumn id="6" xr3:uid="{88C1D531-D327-1544-A671-C5F07A82F946}" name="comments" dataDxfId="98"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{11008CC8-5C85-3B48-82BD-CD830AD3D6DF}" name="Table18" displayName="Table18" ref="A1:M26" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{11008CC8-5C85-3B48-82BD-CD830AD3D6DF}" name="Table18" displayName="Table18" ref="A1:M26" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96">
   <autoFilter ref="A1:M26" xr:uid="{EF08DB4E-0002-F047-8599-404D4BBF8940}"/>
   <tableColumns count="13">
-    <tableColumn id="10" xr3:uid="{65F12D00-08CD-924A-BE4E-9FD2EC7CACF1}" name="*file" dataDxfId="77"/>
-    <tableColumn id="1" xr3:uid="{203C77A6-285B-124C-AF24-A3511F6244F7}" name="*resource" dataDxfId="76"/>
-    <tableColumn id="5" xr3:uid="{2F8C3C4B-0E49-4A4D-AC20-F814AA26DD74}" name="*group" dataDxfId="75"/>
-    <tableColumn id="2" xr3:uid="{42DAC7A2-384A-144A-9BDC-F241D22F7F74}" name="*direction" dataDxfId="74"/>
-    <tableColumn id="3" xr3:uid="{41DCA0FA-BF94-6343-BF46-01D165299C09}" name="*remote" dataDxfId="73"/>
-    <tableColumn id="4" xr3:uid="{15B7721A-4EE3-9847-9C27-38416048A9AE}" name="ip_version" dataDxfId="72"/>
-    <tableColumn id="9" xr3:uid="{0C37575C-3952-904A-B11D-84DC7EE12B0F}" name="icmp.code" dataDxfId="71"/>
-    <tableColumn id="8" xr3:uid="{1CDA1E92-4A45-E742-B2ED-4B8D9670CA18}" name="icmp.type" dataDxfId="70"/>
-    <tableColumn id="7" xr3:uid="{DEE8533C-7DBB-6B4E-95DA-ADF92BBA34C8}" name="tcp.port_min" dataDxfId="69"/>
-    <tableColumn id="6" xr3:uid="{9B67B5CE-A552-3B4B-A870-AA27F074FBE8}" name="tcp.port_max" dataDxfId="68"/>
-    <tableColumn id="12" xr3:uid="{8409EB54-1EA9-6F4A-A691-2C42D27305CF}" name="udp.port_min" dataDxfId="67"/>
-    <tableColumn id="13" xr3:uid="{260B4A5A-5065-9643-BB54-1EF05DDE5EC6}" name="udp.port_max" dataDxfId="66"/>
-    <tableColumn id="11" xr3:uid="{1675F4DC-6C7F-E947-8B75-C5B10333959E}" name="comments" dataDxfId="65"/>
+    <tableColumn id="10" xr3:uid="{65F12D00-08CD-924A-BE4E-9FD2EC7CACF1}" name="*file" dataDxfId="95"/>
+    <tableColumn id="1" xr3:uid="{203C77A6-285B-124C-AF24-A3511F6244F7}" name="*resource" dataDxfId="94"/>
+    <tableColumn id="5" xr3:uid="{2F8C3C4B-0E49-4A4D-AC20-F814AA26DD74}" name="*group" dataDxfId="93"/>
+    <tableColumn id="2" xr3:uid="{42DAC7A2-384A-144A-9BDC-F241D22F7F74}" name="*direction" dataDxfId="92"/>
+    <tableColumn id="3" xr3:uid="{41DCA0FA-BF94-6343-BF46-01D165299C09}" name="*remote" dataDxfId="91"/>
+    <tableColumn id="4" xr3:uid="{15B7721A-4EE3-9847-9C27-38416048A9AE}" name="ip_version" dataDxfId="90"/>
+    <tableColumn id="9" xr3:uid="{0C37575C-3952-904A-B11D-84DC7EE12B0F}" name="icmp.code" dataDxfId="89"/>
+    <tableColumn id="8" xr3:uid="{1CDA1E92-4A45-E742-B2ED-4B8D9670CA18}" name="icmp.type" dataDxfId="88"/>
+    <tableColumn id="7" xr3:uid="{DEE8533C-7DBB-6B4E-95DA-ADF92BBA34C8}" name="tcp.port_min" dataDxfId="87"/>
+    <tableColumn id="6" xr3:uid="{9B67B5CE-A552-3B4B-A870-AA27F074FBE8}" name="tcp.port_max" dataDxfId="86"/>
+    <tableColumn id="12" xr3:uid="{8409EB54-1EA9-6F4A-A691-2C42D27305CF}" name="udp.port_min" dataDxfId="85"/>
+    <tableColumn id="13" xr3:uid="{260B4A5A-5065-9643-BB54-1EF05DDE5EC6}" name="udp.port_max" dataDxfId="84"/>
+    <tableColumn id="11" xr3:uid="{1675F4DC-6C7F-E947-8B75-C5B10333959E}" name="comments" dataDxfId="83"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{48612795-253E-2045-9A1C-B75C9BF5816E}" name="Table111" displayName="Table111" ref="A1:I5" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{48612795-253E-2045-9A1C-B75C9BF5816E}" name="Table111" displayName="Table111" ref="A1:I5" totalsRowShown="0" headerRowDxfId="82" dataDxfId="81">
   <autoFilter ref="A1:I5" xr:uid="{00881A37-2AAB-7345-9099-83242FC8EDEA}"/>
   <tableColumns count="9">
-    <tableColumn id="8" xr3:uid="{B085DC8C-5027-C347-8B02-4C0064110936}" name="*file" dataDxfId="62"/>
-    <tableColumn id="7" xr3:uid="{5391D14C-5D33-5B49-8022-D5255A98F8A7}" name="*resource" dataDxfId="61"/>
-    <tableColumn id="1" xr3:uid="{73198180-EC4B-3448-8FD7-AD7FE682C21E}" name="*name" dataDxfId="60"/>
-    <tableColumn id="6" xr3:uid="{A3F85132-9C0A-074A-AD1C-FC8C58C48C9A}" name="*authentication_algorithm" dataDxfId="59"/>
-    <tableColumn id="2" xr3:uid="{E34718FD-92F0-1A43-80D5-70140F486148}" name="*encryption_algorithm" dataDxfId="58"/>
-    <tableColumn id="3" xr3:uid="{42FD0836-3534-9647-8D8D-7A54E0E1C7AA}" name="*pfs" dataDxfId="57"/>
-    <tableColumn id="4" xr3:uid="{59778D38-F5AC-AC4E-845F-BC7470387817}" name="key_lifetime" dataDxfId="56"/>
-    <tableColumn id="5" xr3:uid="{BABC3429-E57A-4F47-92E7-58CB470AF7F9}" name="resource_group" dataDxfId="55"/>
-    <tableColumn id="9" xr3:uid="{B6FD0690-215F-1D4E-B4EC-214AAB36BD3C}" name="comments" dataDxfId="54"/>
+    <tableColumn id="8" xr3:uid="{B085DC8C-5027-C347-8B02-4C0064110936}" name="*file" dataDxfId="80"/>
+    <tableColumn id="7" xr3:uid="{5391D14C-5D33-5B49-8022-D5255A98F8A7}" name="*resource" dataDxfId="79"/>
+    <tableColumn id="1" xr3:uid="{73198180-EC4B-3448-8FD7-AD7FE682C21E}" name="*name" dataDxfId="78"/>
+    <tableColumn id="6" xr3:uid="{A3F85132-9C0A-074A-AD1C-FC8C58C48C9A}" name="*authentication_algorithm" dataDxfId="77"/>
+    <tableColumn id="2" xr3:uid="{E34718FD-92F0-1A43-80D5-70140F486148}" name="*encryption_algorithm" dataDxfId="76"/>
+    <tableColumn id="3" xr3:uid="{42FD0836-3534-9647-8D8D-7A54E0E1C7AA}" name="*pfs" dataDxfId="75"/>
+    <tableColumn id="4" xr3:uid="{59778D38-F5AC-AC4E-845F-BC7470387817}" name="key_lifetime" dataDxfId="74"/>
+    <tableColumn id="5" xr3:uid="{BABC3429-E57A-4F47-92E7-58CB470AF7F9}" name="resource_group" dataDxfId="73"/>
+    <tableColumn id="9" xr3:uid="{B6FD0690-215F-1D4E-B4EC-214AAB36BD3C}" name="comments" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{EE4FC002-D07C-9447-9703-8452CE1C018E}" name="Table11112" displayName="Table11112" ref="A1:J5" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{EE4FC002-D07C-9447-9703-8452CE1C018E}" name="Table11112" displayName="Table11112" ref="A1:J5" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
   <autoFilter ref="A1:J5" xr:uid="{00881A37-2AAB-7345-9099-83242FC8EDEA}"/>
   <tableColumns count="10">
-    <tableColumn id="9" xr3:uid="{80EAF491-D0BC-DA46-9B6C-B51BD4FA571E}" name="*file" dataDxfId="51"/>
-    <tableColumn id="3" xr3:uid="{605506A1-230A-B34B-AB8A-2448B3FEE895}" name="*resource" dataDxfId="50"/>
-    <tableColumn id="1" xr3:uid="{06812B35-A623-5241-A8DF-8EEB6166846D}" name="*name" dataDxfId="49"/>
-    <tableColumn id="6" xr3:uid="{9551CB52-166F-6E47-9A17-EC3E828FEB2C}" name="*authentication_algorithm" dataDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{246BA229-88CD-0A4B-AD52-5F86AA06873E}" name="*encryption_algorithm" dataDxfId="47"/>
-    <tableColumn id="7" xr3:uid="{2E993777-DA48-4C4D-B929-49BFFB90F9D0}" name="*dh_group" dataDxfId="46"/>
-    <tableColumn id="8" xr3:uid="{A6127979-DB02-954A-BE3A-277928AF4686}" name="ike_version" dataDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{1E691E85-EB8B-A64D-B4A6-22E7A68094F6}" name="key_lifetime" dataDxfId="44"/>
-    <tableColumn id="5" xr3:uid="{9B4820A8-622D-1540-A53E-6FCBAB87C546}" name="resource_group" dataDxfId="43"/>
-    <tableColumn id="10" xr3:uid="{2AF8446C-7F6E-1241-8191-A47FE0FD039A}" name="comments" dataDxfId="42"/>
+    <tableColumn id="9" xr3:uid="{80EAF491-D0BC-DA46-9B6C-B51BD4FA571E}" name="*file" dataDxfId="69"/>
+    <tableColumn id="3" xr3:uid="{605506A1-230A-B34B-AB8A-2448B3FEE895}" name="*resource" dataDxfId="68"/>
+    <tableColumn id="1" xr3:uid="{06812B35-A623-5241-A8DF-8EEB6166846D}" name="*name" dataDxfId="67"/>
+    <tableColumn id="6" xr3:uid="{9551CB52-166F-6E47-9A17-EC3E828FEB2C}" name="*authentication_algorithm" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{246BA229-88CD-0A4B-AD52-5F86AA06873E}" name="*encryption_algorithm" dataDxfId="65"/>
+    <tableColumn id="7" xr3:uid="{2E993777-DA48-4C4D-B929-49BFFB90F9D0}" name="*dh_group" dataDxfId="64"/>
+    <tableColumn id="8" xr3:uid="{A6127979-DB02-954A-BE3A-277928AF4686}" name="ike_version" dataDxfId="63"/>
+    <tableColumn id="4" xr3:uid="{1E691E85-EB8B-A64D-B4A6-22E7A68094F6}" name="key_lifetime" dataDxfId="62"/>
+    <tableColumn id="5" xr3:uid="{9B4820A8-622D-1540-A53E-6FCBAB87C546}" name="resource_group" dataDxfId="61"/>
+    <tableColumn id="10" xr3:uid="{2AF8446C-7F6E-1241-8191-A47FE0FD039A}" name="comments" dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6572AD48-7457-384C-9AEF-EEA28F5B52CA}" name="Table16" displayName="Table16" ref="A1:F5" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6572AD48-7457-384C-9AEF-EEA28F5B52CA}" name="Table16" displayName="Table16" ref="A1:F5" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
   <autoFilter ref="A1:F5" xr:uid="{6D379596-E186-C240-BBB4-B8E74F1D3D56}"/>
   <tableColumns count="6">
-    <tableColumn id="5" xr3:uid="{81C41DB6-4DB4-E647-92D8-7170FEE46256}" name="*file" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{4A1FD022-B67C-4641-BE00-614DB42C1390}" name="*resource" dataDxfId="38"/>
-    <tableColumn id="1" xr3:uid="{5FD29999-A9F5-C549-98A3-DFD2B1437449}" name="*name" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{35CF1270-9B78-4243-98F7-E702702F38FF}" name="*subnet" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{B806F889-718F-584A-ADDF-8A3AD802CDFB}" name="resource_group" dataDxfId="35"/>
-    <tableColumn id="6" xr3:uid="{FDCEE129-41D2-4449-AAED-11FB815198FF}" name="comments" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{81C41DB6-4DB4-E647-92D8-7170FEE46256}" name="*file" dataDxfId="57"/>
+    <tableColumn id="4" xr3:uid="{4A1FD022-B67C-4641-BE00-614DB42C1390}" name="*resource" dataDxfId="56"/>
+    <tableColumn id="1" xr3:uid="{5FD29999-A9F5-C549-98A3-DFD2B1437449}" name="*name" dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{35CF1270-9B78-4243-98F7-E702702F38FF}" name="*subnet" dataDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{B806F889-718F-584A-ADDF-8A3AD802CDFB}" name="resource_group" dataDxfId="53"/>
+    <tableColumn id="6" xr3:uid="{FDCEE129-41D2-4449-AAED-11FB815198FF}" name="comments" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C23E10F9-4BE4-C942-8367-5CE5B9752ED3}" name="Table15" displayName="Table15" ref="A1:P5" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C23E10F9-4BE4-C942-8367-5CE5B9752ED3}" name="Table15" displayName="Table15" ref="A1:P5" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
   <autoFilter ref="A1:P5" xr:uid="{27D8B65D-C3AF-BD4B-8BB7-5754C974B57F}"/>
   <tableColumns count="16">
-    <tableColumn id="15" xr3:uid="{AEA416E1-0B9B-CE41-9B41-923D8909F117}" name="*file" dataDxfId="31"/>
-    <tableColumn id="14" xr3:uid="{77D15CEA-2F6B-5043-873E-DDC8A59F18E1}" name="*resource" dataDxfId="30"/>
-    <tableColumn id="1" xr3:uid="{C4B8842B-2BB7-EB49-B6D2-B6721C54DC5F}" name="*name" dataDxfId="29"/>
-    <tableColumn id="13" xr3:uid="{78EC6C87-C780-E34D-BBD5-54ED244AB6D6}" name="*vpn_gateway" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{DBBB9AC2-20E7-974C-935D-20C40D819A02}" name="*peer_address" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{5CDA888D-9763-CE46-98E3-D4B85974B5A5}" name="*preshared_key" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{D1C2C80B-E944-E049-AD39-98867623465E}" name="local_cidrs" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{B6F5AA94-6774-DA4F-8D22-7820C9CFB052}" name="peer_cidrs" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{A49490F8-FF19-4247-A9DC-3E9A8C9508D2}" name="admin_state_up" dataDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{D393C6C1-4F72-964B-9D76-BE2A1539821D}" name="action" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{D523FCFB-A055-084E-B6ED-C788AB1D158E}" name="interval" dataDxfId="21"/>
-    <tableColumn id="9" xr3:uid="{9A0739C3-7687-E94A-984F-5C145DFE3E89}" name="timeout" dataDxfId="20"/>
-    <tableColumn id="10" xr3:uid="{ACD56801-B98E-7847-85C3-F2FFBA76F061}" name="ike_policy" dataDxfId="19"/>
-    <tableColumn id="11" xr3:uid="{1BD10945-B68C-DF4E-AA5E-ACEC66F06E3C}" name="ipsec_policy" dataDxfId="18"/>
-    <tableColumn id="12" xr3:uid="{4B0694AF-1BD1-694F-90B1-B1A9567550B0}" name="timeout.delete" dataDxfId="17"/>
-    <tableColumn id="16" xr3:uid="{D2BE25AD-482C-2448-893C-520E3FFC0012}" name="comments" dataDxfId="16"/>
+    <tableColumn id="15" xr3:uid="{AEA416E1-0B9B-CE41-9B41-923D8909F117}" name="*file" dataDxfId="49"/>
+    <tableColumn id="14" xr3:uid="{77D15CEA-2F6B-5043-873E-DDC8A59F18E1}" name="*resource" dataDxfId="48"/>
+    <tableColumn id="1" xr3:uid="{C4B8842B-2BB7-EB49-B6D2-B6721C54DC5F}" name="*name" dataDxfId="47"/>
+    <tableColumn id="13" xr3:uid="{78EC6C87-C780-E34D-BBD5-54ED244AB6D6}" name="*vpn_gateway" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{DBBB9AC2-20E7-974C-935D-20C40D819A02}" name="*peer_address" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{5CDA888D-9763-CE46-98E3-D4B85974B5A5}" name="*preshared_key" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{D1C2C80B-E944-E049-AD39-98867623465E}" name="local_cidrs" dataDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{B6F5AA94-6774-DA4F-8D22-7820C9CFB052}" name="peer_cidrs" dataDxfId="42"/>
+    <tableColumn id="6" xr3:uid="{A49490F8-FF19-4247-A9DC-3E9A8C9508D2}" name="admin_state_up" dataDxfId="41"/>
+    <tableColumn id="7" xr3:uid="{D393C6C1-4F72-964B-9D76-BE2A1539821D}" name="action" dataDxfId="40"/>
+    <tableColumn id="8" xr3:uid="{D523FCFB-A055-084E-B6ED-C788AB1D158E}" name="interval" dataDxfId="39"/>
+    <tableColumn id="9" xr3:uid="{9A0739C3-7687-E94A-984F-5C145DFE3E89}" name="timeout" dataDxfId="38"/>
+    <tableColumn id="10" xr3:uid="{ACD56801-B98E-7847-85C3-F2FFBA76F061}" name="ike_policy" dataDxfId="37"/>
+    <tableColumn id="11" xr3:uid="{1BD10945-B68C-DF4E-AA5E-ACEC66F06E3C}" name="ipsec_policy" dataDxfId="36"/>
+    <tableColumn id="12" xr3:uid="{4B0694AF-1BD1-694F-90B1-B1A9567550B0}" name="timeout.delete" dataDxfId="35"/>
+    <tableColumn id="16" xr3:uid="{D2BE25AD-482C-2448-893C-520E3FFC0012}" name="comments" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{66B01468-17B1-DF49-BD45-B84826DE910D}" name="Table32" displayName="Table32" ref="A1:G4" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="A1:G4" xr:uid="{E53C9C86-FACA-2C40-85AF-B9BA3559B380}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{FBE293FA-80EC-F242-887C-B11422C1022D}" name="Table169" displayName="Table169" ref="A1:G5" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A1:G5" xr:uid="{6D379596-E186-C240-BBB4-B8E74F1D3D56}"/>
   <tableColumns count="7">
-    <tableColumn id="6" xr3:uid="{8F21586E-BECB-3F45-BEAA-A449A14BE047}" name="*file" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{4EF03EBF-5996-424F-93A5-4447C7F1B426}" name="*resource" dataDxfId="12"/>
-    <tableColumn id="1" xr3:uid="{C065294C-9139-324E-B19B-962D20BC4BE9}" name="*name" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{592C42FA-35FC-334C-9912-6BAE32344BD6}" name="*public_key" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{A36A827B-73DB-0749-B08B-5E9FBF4CF71C}" name="resource_group" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{F6CE2A63-DCA4-AB46-AD6C-B729704A5EAC}" name="tags" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{461DC722-A60D-2D4E-8D06-0C3D76DA4F10}" name="comments" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{1783CBE2-5818-4D4F-8A50-0D325E64887E}" name="*file" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{7D27F76A-C057-7B41-8211-3A3FA8658B48}" name="*resource" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{7E6DC40E-F6C9-C643-8520-0BEA365DF21F}" name="*name" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{F1EC0EF8-857C-F845-8233-1A4645A1D255}" name="*global" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{71D8A097-A059-D544-88DD-CC2EB82698A3}" name="location" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{7C954070-A47C-BC40-B8B7-36A3A762A9FF}" name="resource_group" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{9825ACF3-765C-1A4C-8ED3-664BBDA75427}" name="comments" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E8C732A8-0017-264D-8362-11409D4ADB8A}" name="Table329" displayName="Table329" ref="A1:E5" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E5" xr:uid="{853761A8-3C8D-D146-AF16-A9CD69B737CB}"/>
-  <tableColumns count="5">
-    <tableColumn id="6" xr3:uid="{C7B59D49-52B4-E74B-980A-CBAA1960F9B9}" name="*file" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{0F8D8265-8F60-6746-958A-BB70EE098749}" name="*resource" dataDxfId="3"/>
-    <tableColumn id="1" xr3:uid="{20125E38-3425-9540-8E50-F8247EA67681}" name="*name" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{50B39641-31D5-1A42-A833-F3F591AE4879}" name="tags" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{E9307884-D588-8840-BA44-7ABC5CDEF259}" name="comments" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{7FF21D0D-5BB2-7147-81F3-634B6BBC66AE}" name="Table16910" displayName="Table16910" ref="A1:G5" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:G5" xr:uid="{6D379596-E186-C240-BBB4-B8E74F1D3D56}"/>
+  <tableColumns count="7">
+    <tableColumn id="5" xr3:uid="{E861A381-AFF9-CC4F-88E6-39905BA5EA5A}" name="*file" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{7EDBEE7E-8A29-A44F-B042-967D4F2FFCC7}" name="*resource" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{6F7F1276-5372-6340-899C-BF0D347BEE24}" name="name" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{1C7A2F6D-A0B2-C347-BF50-233D0B3D59D4}" name="*gateway" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{50AFBAF0-B636-BA4C-AB12-FA8E8220FEC3}" name="*network_type" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{17DC867E-74AA-2A43-B864-99A770207616}" name="network_id" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{32EB9F06-C8B0-8440-BEC7-F21EB35097EC}" name="comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2548,6 +2698,177 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B645F3C-DBF6-5F4F-ABFE-BBA299212CDA}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8986B38C-6E3F-B448-9CAD-8CBE86D28040}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F29E99F-EAC6-EF42-BBDE-1489EAD1BB17}">
   <dimension ref="A1:H8"/>
@@ -4049,67 +4370,59 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B645F3C-DBF6-5F4F-ABFE-BBA299212CDA}">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3B141E-E592-5D47-A012-492F5D4BE721}">
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.83203125" customWidth="1"/>
+    <col min="13" max="13" width="18.83203125" customWidth="1"/>
+    <col min="14" max="14" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="D1" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="9" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>98</v>
-      </c>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4117,8 +4430,15 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -4126,6 +4446,20 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4136,80 +4470,96 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8986B38C-6E3F-B448-9CAD-8CBE86D28040}">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14EDADE6-A3E3-3B42-BD38-CD2F83BE556A}">
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.83203125" customWidth="1"/>
+    <col min="13" max="13" width="18.83203125" customWidth="1"/>
+    <col min="14" max="14" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="C1" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>132</v>
-      </c>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>135</v>
-      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>